<commit_message>
bugfix for attack village
</commit_message>
<xml_diff>
--- a/gameData/shared/AllianceVillage.xlsx
+++ b/gameData/shared/AllianceVillage.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="8440" yWindow="3340" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="5"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="7">
   <si>
     <t>INT_level</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -51,14 +51,6 @@
   </si>
   <si>
     <t>INT_needHonour</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>STR_soldiers</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>redDragon_1_5,swordsman_1_10,sentinel_1_10,ranger_1_10</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -859,10 +851,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -873,7 +865,7 @@
     <col min="5" max="16384" width="20.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="15">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -886,11 +878,8 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15">
+    </row>
+    <row r="2" spans="1:4" ht="15">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -903,11 +892,8 @@
       <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="15">
+    </row>
+    <row r="3" spans="1:4" ht="15">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -920,11 +906,8 @@
       <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15">
+    </row>
+    <row r="4" spans="1:4" ht="15">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -937,11 +920,8 @@
       <c r="D4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15">
+    </row>
+    <row r="5" spans="1:4" ht="15">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -954,11 +934,8 @@
       <c r="D5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15">
+    </row>
+    <row r="6" spans="1:4" ht="15">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -971,11 +948,8 @@
       <c r="D6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15">
+    </row>
+    <row r="7" spans="1:4" ht="15">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -988,11 +962,8 @@
       <c r="D7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15">
+    </row>
+    <row r="8" spans="1:4" ht="15">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1005,11 +976,8 @@
       <c r="D8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15">
+    </row>
+    <row r="9" spans="1:4" ht="15">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1022,11 +990,8 @@
       <c r="D9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="15">
+    </row>
+    <row r="10" spans="1:4" ht="15">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1039,11 +1004,8 @@
       <c r="D10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="15">
+    </row>
+    <row r="11" spans="1:4" ht="15">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1056,23 +1018,20 @@
       <c r="D11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="15">
+    </row>
+    <row r="12" spans="1:4" ht="15">
       <c r="C12" s="4"/>
     </row>
-    <row r="13" spans="1:5" ht="15">
+    <row r="13" spans="1:4" ht="15">
       <c r="C13" s="4"/>
     </row>
-    <row r="14" spans="1:5" ht="15">
+    <row r="14" spans="1:4" ht="15">
       <c r="C14" s="4"/>
     </row>
-    <row r="15" spans="1:5" ht="15">
+    <row r="15" spans="1:4" ht="15">
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:5" ht="15">
+    <row r="16" spans="1:4" ht="15">
       <c r="C16" s="4"/>
     </row>
     <row r="17" spans="1:3" ht="15">
@@ -1172,7 +1131,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="E1" sqref="E1:E1048576"/>
@@ -1186,7 +1145,7 @@
     <col min="5" max="16384" width="20.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="15">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1199,11 +1158,8 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15">
+    </row>
+    <row r="2" spans="1:4" ht="15">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1216,11 +1172,8 @@
       <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="15">
+    </row>
+    <row r="3" spans="1:4" ht="15">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1233,11 +1186,8 @@
       <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15">
+    </row>
+    <row r="4" spans="1:4" ht="15">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1250,11 +1200,8 @@
       <c r="D4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15">
+    </row>
+    <row r="5" spans="1:4" ht="15">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1267,11 +1214,8 @@
       <c r="D5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15">
+    </row>
+    <row r="6" spans="1:4" ht="15">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1284,11 +1228,8 @@
       <c r="D6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15">
+    </row>
+    <row r="7" spans="1:4" ht="15">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1301,11 +1242,8 @@
       <c r="D7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15">
+    </row>
+    <row r="8" spans="1:4" ht="15">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1318,11 +1256,8 @@
       <c r="D8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15">
+    </row>
+    <row r="9" spans="1:4" ht="15">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1335,11 +1270,8 @@
       <c r="D9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="15">
+    </row>
+    <row r="10" spans="1:4" ht="15">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1352,11 +1284,8 @@
       <c r="D10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="15">
+    </row>
+    <row r="11" spans="1:4" ht="15">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1369,23 +1298,20 @@
       <c r="D11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="15">
+    </row>
+    <row r="12" spans="1:4" ht="15">
       <c r="C12" s="4"/>
     </row>
-    <row r="13" spans="1:5" ht="15">
+    <row r="13" spans="1:4" ht="15">
       <c r="C13" s="4"/>
     </row>
-    <row r="14" spans="1:5" ht="15">
+    <row r="14" spans="1:4" ht="15">
       <c r="C14" s="4"/>
     </row>
-    <row r="15" spans="1:5" ht="15">
+    <row r="15" spans="1:4" ht="15">
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:5" ht="15">
+    <row r="16" spans="1:4" ht="15">
       <c r="C16" s="4"/>
     </row>
     <row r="17" spans="1:3" ht="15">
@@ -1485,7 +1411,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="E1" sqref="E1:E1048576"/>
@@ -1499,7 +1425,7 @@
     <col min="5" max="16384" width="20.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="15">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1512,11 +1438,8 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15">
+    </row>
+    <row r="2" spans="1:4" ht="15">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1529,11 +1452,8 @@
       <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="15">
+    </row>
+    <row r="3" spans="1:4" ht="15">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1546,11 +1466,8 @@
       <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15">
+    </row>
+    <row r="4" spans="1:4" ht="15">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1563,11 +1480,8 @@
       <c r="D4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15">
+    </row>
+    <row r="5" spans="1:4" ht="15">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1580,11 +1494,8 @@
       <c r="D5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15">
+    </row>
+    <row r="6" spans="1:4" ht="15">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1597,11 +1508,8 @@
       <c r="D6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15">
+    </row>
+    <row r="7" spans="1:4" ht="15">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1614,11 +1522,8 @@
       <c r="D7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15">
+    </row>
+    <row r="8" spans="1:4" ht="15">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1631,11 +1536,8 @@
       <c r="D8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15">
+    </row>
+    <row r="9" spans="1:4" ht="15">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1648,11 +1550,8 @@
       <c r="D9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="15">
+    </row>
+    <row r="10" spans="1:4" ht="15">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1665,11 +1564,8 @@
       <c r="D10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="15">
+    </row>
+    <row r="11" spans="1:4" ht="15">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1682,23 +1578,20 @@
       <c r="D11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="15">
+    </row>
+    <row r="12" spans="1:4" ht="15">
       <c r="C12" s="4"/>
     </row>
-    <row r="13" spans="1:5" ht="15">
+    <row r="13" spans="1:4" ht="15">
       <c r="C13" s="4"/>
     </row>
-    <row r="14" spans="1:5" ht="15">
+    <row r="14" spans="1:4" ht="15">
       <c r="C14" s="4"/>
     </row>
-    <row r="15" spans="1:5" ht="15">
+    <row r="15" spans="1:4" ht="15">
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:5" ht="15">
+    <row r="16" spans="1:4" ht="15">
       <c r="C16" s="4"/>
     </row>
     <row r="17" spans="1:3" ht="15">
@@ -1798,7 +1691,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="E1" sqref="E1:E1048576"/>
@@ -1812,7 +1705,7 @@
     <col min="5" max="16384" width="20.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="15">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1825,11 +1718,8 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15">
+    </row>
+    <row r="2" spans="1:4" ht="15">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1842,11 +1732,8 @@
       <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="15">
+    </row>
+    <row r="3" spans="1:4" ht="15">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1859,11 +1746,8 @@
       <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15">
+    </row>
+    <row r="4" spans="1:4" ht="15">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1876,11 +1760,8 @@
       <c r="D4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15">
+    </row>
+    <row r="5" spans="1:4" ht="15">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1893,11 +1774,8 @@
       <c r="D5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15">
+    </row>
+    <row r="6" spans="1:4" ht="15">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1910,11 +1788,8 @@
       <c r="D6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15">
+    </row>
+    <row r="7" spans="1:4" ht="15">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1927,11 +1802,8 @@
       <c r="D7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15">
+    </row>
+    <row r="8" spans="1:4" ht="15">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1944,11 +1816,8 @@
       <c r="D8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15">
+    </row>
+    <row r="9" spans="1:4" ht="15">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1961,11 +1830,8 @@
       <c r="D9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="15">
+    </row>
+    <row r="10" spans="1:4" ht="15">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1978,11 +1844,8 @@
       <c r="D10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="15">
+    </row>
+    <row r="11" spans="1:4" ht="15">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1995,23 +1858,20 @@
       <c r="D11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="15">
+    </row>
+    <row r="12" spans="1:4" ht="15">
       <c r="C12" s="4"/>
     </row>
-    <row r="13" spans="1:5" ht="15">
+    <row r="13" spans="1:4" ht="15">
       <c r="C13" s="4"/>
     </row>
-    <row r="14" spans="1:5" ht="15">
+    <row r="14" spans="1:4" ht="15">
       <c r="C14" s="4"/>
     </row>
-    <row r="15" spans="1:5" ht="15">
+    <row r="15" spans="1:4" ht="15">
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:5" ht="15">
+    <row r="16" spans="1:4" ht="15">
       <c r="C16" s="4"/>
     </row>
     <row r="17" spans="1:3" ht="15">
@@ -2111,7 +1971,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="E1" sqref="E1:E1048576"/>
@@ -2125,7 +1985,7 @@
     <col min="5" max="16384" width="20.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="15">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2138,11 +1998,8 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15">
+    </row>
+    <row r="2" spans="1:4" ht="15">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2155,11 +2012,8 @@
       <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="15">
+    </row>
+    <row r="3" spans="1:4" ht="15">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2172,11 +2026,8 @@
       <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15">
+    </row>
+    <row r="4" spans="1:4" ht="15">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2189,11 +2040,8 @@
       <c r="D4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15">
+    </row>
+    <row r="5" spans="1:4" ht="15">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2206,11 +2054,8 @@
       <c r="D5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15">
+    </row>
+    <row r="6" spans="1:4" ht="15">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2223,11 +2068,8 @@
       <c r="D6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15">
+    </row>
+    <row r="7" spans="1:4" ht="15">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -2240,11 +2082,8 @@
       <c r="D7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15">
+    </row>
+    <row r="8" spans="1:4" ht="15">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -2257,11 +2096,8 @@
       <c r="D8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15">
+    </row>
+    <row r="9" spans="1:4" ht="15">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -2274,11 +2110,8 @@
       <c r="D9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="15">
+    </row>
+    <row r="10" spans="1:4" ht="15">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -2291,11 +2124,8 @@
       <c r="D10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="15">
+    </row>
+    <row r="11" spans="1:4" ht="15">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -2308,23 +2138,20 @@
       <c r="D11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="15">
+    </row>
+    <row r="12" spans="1:4" ht="15">
       <c r="C12" s="4"/>
     </row>
-    <row r="13" spans="1:5" ht="15">
+    <row r="13" spans="1:4" ht="15">
       <c r="C13" s="4"/>
     </row>
-    <row r="14" spans="1:5" ht="15">
+    <row r="14" spans="1:4" ht="15">
       <c r="C14" s="4"/>
     </row>
-    <row r="15" spans="1:5" ht="15">
+    <row r="15" spans="1:4" ht="15">
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:5" ht="15">
+    <row r="16" spans="1:4" ht="15">
       <c r="C16" s="4"/>
     </row>
     <row r="17" spans="1:3" ht="15">
@@ -2424,10 +2251,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -2438,7 +2265,7 @@
     <col min="4" max="16384" width="20.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="15">
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2448,11 +2275,8 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15">
+    </row>
+    <row r="2" spans="1:3" ht="15">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2462,11 +2286,8 @@
       <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15">
+    </row>
+    <row r="3" spans="1:3" ht="15">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2476,11 +2297,8 @@
       <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15">
+    </row>
+    <row r="4" spans="1:3" ht="15">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2490,11 +2308,8 @@
       <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15">
+    </row>
+    <row r="5" spans="1:3" ht="15">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2504,11 +2319,8 @@
       <c r="C5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15">
+    </row>
+    <row r="6" spans="1:3" ht="15">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2518,11 +2330,8 @@
       <c r="C6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15">
+    </row>
+    <row r="7" spans="1:3" ht="15">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -2532,11 +2341,8 @@
       <c r="C7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15">
+    </row>
+    <row r="8" spans="1:3" ht="15">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -2546,11 +2352,8 @@
       <c r="C8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15">
+    </row>
+    <row r="9" spans="1:3" ht="15">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -2560,11 +2363,8 @@
       <c r="C9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="15">
+    </row>
+    <row r="10" spans="1:3" ht="15">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -2574,11 +2374,8 @@
       <c r="C10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="15">
+    </row>
+    <row r="11" spans="1:3" ht="15">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -2588,23 +2385,20 @@
       <c r="C11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="15">
+    </row>
+    <row r="12" spans="1:3" ht="15">
       <c r="B12" s="4"/>
     </row>
-    <row r="13" spans="1:4" ht="15">
+    <row r="13" spans="1:3" ht="15">
       <c r="B13" s="4"/>
     </row>
-    <row r="14" spans="1:4" ht="15">
+    <row r="14" spans="1:3" ht="15">
       <c r="B14" s="4"/>
     </row>
-    <row r="15" spans="1:4" ht="15">
+    <row r="15" spans="1:3" ht="15">
       <c r="B15" s="4"/>
     </row>
-    <row r="16" spans="1:4" ht="15">
+    <row r="16" spans="1:3" ht="15">
       <c r="B16" s="4"/>
     </row>
     <row r="17" spans="1:2" ht="15">

</xml_diff>